<commit_message>
[C] enum 값 최신화
</commit_message>
<xml_diff>
--- a/AtServerEngine/Data/Character/Character.xlsx
+++ b/AtServerEngine/Data/Character/Character.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ath331\Desktop\a\VisualStudio\C++\AtServerEngine\Data\Character\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ath331\Desktop\a\Game\T_Survivor\AtServerEngine\Data\Character\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56C3BF8-0C64-4662-9C2A-C17DF5E3AC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D5DE1C-066E-4F9F-B283-44823992A309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4455" yWindow="2715" windowWidth="28800" windowHeight="15885" xr2:uid="{63715C51-116E-4948-BF31-B1B087F565B5}"/>
+    <workbookView xWindow="7410" yWindow="1590" windowWidth="28800" windowHeight="15885" xr2:uid="{63715C51-116E-4948-BF31-B1B087F565B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Character" sheetId="1" r:id="rId1"/>
@@ -58,18 +58,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Equipment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Etc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Useable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>*SC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -95,6 +83,18 @@
   </si>
   <si>
     <t>Disable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BAG_TYPE_EQUIPMENT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BAG_TYPE_ETC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BAG_TYPE_USEABLE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -564,14 +564,14 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.625" customWidth="1"/>
     <col min="2" max="3" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -580,10 +580,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>0</v>
@@ -591,21 +591,21 @@
     </row>
     <row r="2" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -622,10 +622,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -639,7 +639,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
@@ -653,7 +653,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
@@ -664,7 +664,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.3"/>

</xml_diff>